<commit_message>
Added new WP3 IDs
</commit_message>
<xml_diff>
--- a/Code Lists/ToopDocumentTypeIdentifiers-v2.xlsx
+++ b/Code Lists/ToopDocumentTypeIdentifiers-v2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="_ftnref3" localSheetId="0">'Document Type'!$A$3</definedName>
     <definedName name="_ftnref4" localSheetId="0">'Document Type'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Common Name</t>
   </si>
@@ -55,13 +55,64 @@
   </si>
   <si>
     <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.registeredorganization::1.40</t>
+  </si>
+  <si>
+    <t>Ship Certificate</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.shipcertificate-list::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.shipcertificate::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.shipcertificate::1.40</t>
+  </si>
+  <si>
+    <t>Crew Certificate</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.crewcertificate::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.registeredorganization-list::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.registeredorganization-list::1.40</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.evidence-list::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.evidence-list::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.evidence::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.evidence::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.shipcertificate-list::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.crewcertificate-list::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.crewcertificate-list::1.40</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.crewcertificate::1.40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -128,14 +179,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,32 +600,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="6" customWidth="1"/>
+    <col min="2" max="2" width="94" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="1"/>
+    <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -575,11 +635,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1">
@@ -593,11 +653,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1">
@@ -611,11 +671,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
@@ -626,17 +686,257 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5">
+        <v>2</v>
+      </c>
+      <c r="D21" s="5" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added "List" to display name of certain document types
</commit_message>
<xml_diff>
--- a/Code Lists/ToopDocumentTypeIdentifiers-v2.xlsx
+++ b/Code Lists/ToopDocumentTypeIdentifiers-v2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="_ftnref3" localSheetId="0">'Document Type'!$A$3</definedName>
     <definedName name="_ftnref4" localSheetId="0">'Document Type'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Common Name</t>
   </si>
@@ -106,13 +106,25 @@
   </si>
   <si>
     <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.crewcertificate::1.40</t>
+  </si>
+  <si>
+    <t>Crew Certificate List</t>
+  </si>
+  <si>
+    <t>Ship Certificate List</t>
+  </si>
+  <si>
+    <t>Registered Organization List</t>
+  </si>
+  <si>
+    <t>Evidence List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,25 +612,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23" style="6" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" style="6" customWidth="1"/>
     <col min="2" max="2" width="94" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -635,7 +647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -653,7 +665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -671,9 +683,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>16</v>
@@ -686,9 +698,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>17</v>
@@ -701,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -716,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -731,9 +743,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>23</v>
@@ -746,9 +758,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>11</v>
@@ -761,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -776,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -791,9 +803,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>24</v>
@@ -806,9 +818,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>25</v>
@@ -821,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -836,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
@@ -851,9 +863,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>19</v>
@@ -866,9 +878,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>20</v>
@@ -881,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -896,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Added "Request" and "Response" to display names
</commit_message>
<xml_diff>
--- a/Code Lists/ToopDocumentTypeIdentifiers-v2.xlsx
+++ b/Code Lists/ToopDocumentTypeIdentifiers-v2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Common Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>urn:eu:toop:ns:dataexchange-1p10::Request##urn:eu.toop.request.registeredorganization::1.10</t>
   </si>
   <si>
-    <t>Registered Organization</t>
-  </si>
-  <si>
     <t>urn:eu:toop:ns:dataexchange-1p10::Response##urn:eu.toop.response.registeredorganization::1.10</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.registeredorganization::1.40</t>
   </si>
   <si>
-    <t>Ship Certificate</t>
-  </si>
-  <si>
     <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.shipcertificate-list::1.40</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.shipcertificate::1.40</t>
   </si>
   <si>
-    <t>Crew Certificate</t>
-  </si>
-  <si>
     <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.crewcertificate::1.40</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.registeredorganization-list::1.40</t>
   </si>
   <si>
-    <t>Evidence</t>
-  </si>
-  <si>
     <t>urn:eu:toop:ns:dataexchange-1p40::Request##urn:eu.toop.request.evidence-list::1.40</t>
   </si>
   <si>
@@ -108,16 +96,52 @@
     <t>urn:eu:toop:ns:dataexchange-1p40::Response##urn:eu.toop.response.crewcertificate::1.40</t>
   </si>
   <si>
-    <t>Crew Certificate List</t>
-  </si>
-  <si>
-    <t>Ship Certificate List</t>
-  </si>
-  <si>
-    <t>Registered Organization List</t>
-  </si>
-  <si>
-    <t>Evidence List</t>
+    <t>Registered Organization Request</t>
+  </si>
+  <si>
+    <t>Registered Organization Response</t>
+  </si>
+  <si>
+    <t>Registered Organization List Request</t>
+  </si>
+  <si>
+    <t>Registered Organization List Response</t>
+  </si>
+  <si>
+    <t>Ship Certificate List Request</t>
+  </si>
+  <si>
+    <t>Ship Certificate List Response</t>
+  </si>
+  <si>
+    <t>Ship Certificate Request</t>
+  </si>
+  <si>
+    <t>Ship Certificate Response</t>
+  </si>
+  <si>
+    <t>Crew Certificate List Request</t>
+  </si>
+  <si>
+    <t>Crew Certificate List Response</t>
+  </si>
+  <si>
+    <t>Crew Certificate Request</t>
+  </si>
+  <si>
+    <t>Crew Certificate Response</t>
+  </si>
+  <si>
+    <t>Evidence List Request</t>
+  </si>
+  <si>
+    <t>Evidence List Response</t>
+  </si>
+  <si>
+    <t>Evidence Request</t>
+  </si>
+  <si>
+    <t>Evidence Response</t>
   </si>
 </sst>
 </file>
@@ -617,7 +641,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -635,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -649,7 +673,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
@@ -667,10 +691,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -685,10 +709,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
@@ -700,10 +724,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5">
         <v>2</v>
@@ -715,10 +739,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
@@ -730,10 +754,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
@@ -745,10 +769,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5">
         <v>2</v>
@@ -763,7 +787,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
@@ -775,10 +799,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
@@ -790,10 +814,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="5">
         <v>2</v>
@@ -805,10 +829,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
@@ -820,10 +844,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5">
         <v>2</v>
@@ -835,10 +859,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14" s="5">
         <v>2</v>
@@ -850,10 +874,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5">
         <v>2</v>
@@ -865,10 +889,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C16" s="5">
         <v>2</v>
@@ -880,10 +904,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C17" s="5">
         <v>2</v>
@@ -895,10 +919,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5">
         <v>2</v>
@@ -910,10 +934,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="C19" s="5">
         <v>2</v>

</xml_diff>